<commit_message>
simpler model. Let's start from beginning and then complicate more the code
</commit_message>
<xml_diff>
--- a/EDF_4_grid_v9.xlsx
+++ b/EDF_4_grid_v9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Engenharia Eletrotécnica\Doutoramento\1º Ano\Tese\Modelação\Redes de teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\laris\ev4eu_algorithms\opt_communities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139EA0F6-00BD-4774-973C-665B1F8DDC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A644504-7107-478D-8039-8193C7256A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralInfo" sheetId="5" r:id="rId1"/>
@@ -1363,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -13094,8 +13094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C493CC03-2EEE-4C38-B4EF-000782EAEF79}">
   <dimension ref="A1:AD31"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A31"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13779,7 +13779,7 @@
         <v>39</v>
       </c>
       <c r="D9" s="10">
-        <v>100000</v>
+        <v>100</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>30</v>

</xml_diff>